<commit_message>
excel des masse rempli avec les prévisions
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/Masse Elec.xlsx
+++ b/EL - Electrical/Autre/Masse Elec.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC2746A-A656-4D86-BADC-5B6D5AFC90B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA89CE37-0FEB-4751-90BA-9B62435F22C9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOTAL" sheetId="1" r:id="rId1"/>
@@ -16,8 +16,9 @@
     <sheet name="Câble faisceau avant" sheetId="3" r:id="rId6"/>
     <sheet name="Power box" sheetId="4" r:id="rId7"/>
     <sheet name="Télémétrie" sheetId="8" r:id="rId8"/>
-    <sheet name="Autre" sheetId="9" r:id="rId9"/>
-    <sheet name="Visserie" sheetId="10" r:id="rId10"/>
+    <sheet name="Autres" sheetId="9" r:id="rId9"/>
+    <sheet name="Passage de vitesse" sheetId="11" r:id="rId10"/>
+    <sheet name="Visserie" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="103">
   <si>
     <t>Pièce</t>
   </si>
@@ -200,12 +201,153 @@
   </si>
   <si>
     <t>Visserie</t>
+  </si>
+  <si>
+    <t>Master switch</t>
+  </si>
+  <si>
+    <t>Support master switch</t>
+  </si>
+  <si>
+    <t>Sonde lambda</t>
+  </si>
+  <si>
+    <t>Capteur de vitesse</t>
+  </si>
+  <si>
+    <t>Break light</t>
+  </si>
+  <si>
+    <t>Regulateur</t>
+  </si>
+  <si>
+    <t>Passage de vitesse</t>
+  </si>
+  <si>
+    <t>Servomoteur</t>
+  </si>
+  <si>
+    <t>Câble</t>
+  </si>
+  <si>
+    <t>Boîte</t>
+  </si>
+  <si>
+    <t>Carte électronique</t>
+  </si>
+  <si>
+    <t>DTA</t>
+  </si>
+  <si>
+    <t>Relai démarrage</t>
+  </si>
+  <si>
+    <t>Boitier lambda</t>
+  </si>
+  <si>
+    <t>Boitier</t>
+  </si>
+  <si>
+    <t>Relais</t>
+  </si>
+  <si>
+    <t>Fusible</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>boulon M3 TDB</t>
+  </si>
+  <si>
+    <t>boulon M3 Master switch</t>
+  </si>
+  <si>
+    <t>boulon M3 Power box</t>
+  </si>
+  <si>
+    <t>Boulon M4 masse ??</t>
+  </si>
+  <si>
+    <t>8STA71699SD</t>
+  </si>
+  <si>
+    <t>8STA6199PD</t>
+  </si>
+  <si>
+    <t>8STA70635SA</t>
+  </si>
+  <si>
+    <t>8STA60635PA</t>
+  </si>
+  <si>
+    <t>8STA01497PB</t>
+  </si>
+  <si>
+    <t>8STA61497SB</t>
+  </si>
+  <si>
+    <t>8STA01497SN</t>
+  </si>
+  <si>
+    <t>8STA61497PN</t>
+  </si>
+  <si>
+    <t>8STA01035SD</t>
+  </si>
+  <si>
+    <t>8STA61035PD</t>
+  </si>
+  <si>
+    <t>8STA00201SN</t>
+  </si>
+  <si>
+    <t>8STA60201PN</t>
+  </si>
+  <si>
+    <t>8STA00435SA</t>
+  </si>
+  <si>
+    <t>8STA60435PA</t>
+  </si>
+  <si>
+    <t>8STA01035SN</t>
+  </si>
+  <si>
+    <t>8STA61035PN</t>
+  </si>
+  <si>
+    <t>8STA10235D</t>
+  </si>
+  <si>
+    <t>8STA60235D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batterie </t>
+  </si>
+  <si>
+    <t>Support Batterie</t>
+  </si>
+  <si>
+    <t>Boulon M4 Batterie ??</t>
+  </si>
+  <si>
+    <t>Boitier contrôleur</t>
+  </si>
+  <si>
+    <t>Carte avant</t>
+  </si>
+  <si>
+    <t>Autres (DTA, Batterie..)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -270,7 +412,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,8 +431,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D18E"/>
+        <bgColor rgb="FFC5E0B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE699"/>
+        <bgColor rgb="FFFFD966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9DC3E6"/>
+        <bgColor rgb="FFBDD7EE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4B183"/>
+        <bgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -444,11 +616,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -470,9 +694,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -532,11 +753,107 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="30">
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <border outline="0">
         <top style="medium">
@@ -1107,35 +1424,1552 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TOTAL!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Masse prévisionelle (kg)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-C149-455F-928B-59C6D903BA17}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-C149-455F-928B-59C6D903BA17}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-C149-455F-928B-59C6D903BA17}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-C149-455F-928B-59C6D903BA17}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-C149-455F-928B-59C6D903BA17}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-C149-455F-928B-59C6D903BA17}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-C149-455F-928B-59C6D903BA17}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-C149-455F-928B-59C6D903BA17}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-C149-455F-928B-59C6D903BA17}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-C149-455F-928B-59C6D903BA17}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-C149-455F-928B-59C6D903BA17}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-C149-455F-928B-59C6D903BA17}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-C149-455F-928B-59C6D903BA17}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-C149-455F-928B-59C6D903BA17}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent5"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-C149-455F-928B-59C6D903BA17}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent6"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-C149-455F-928B-59C6D903BA17}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1">
+                          <a:lumMod val="60000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-C149-455F-928B-59C6D903BA17}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2">
+                          <a:lumMod val="60000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-C149-455F-928B-59C6D903BA17}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3">
+                          <a:lumMod val="60000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-C149-455F-928B-59C6D903BA17}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4">
+                          <a:lumMod val="60000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-C149-455F-928B-59C6D903BA17}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>TOTAL!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Chapes</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tableau de bord</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Connecteur</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Câbles faisceau arrière</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Câbles faisceau avant</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Power box</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Télémétrie</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Autres (DTA, Batterie..)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Visserie</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Passage de vitesse</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TOTAL!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.11100000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0020000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.000">
+                  <c:v>0.55620000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71500000000000008</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.8790000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.14499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4000000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C149-455F-928B-59C6D903BA17}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="259">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="10000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d>
+        <a:bevelT w="127000" h="127000"/>
+        <a:bevelB w="127000" h="127000"/>
+      </a:sp3d>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F14A8E9-810F-4FA5-8FFB-20D300D8AFAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BB731EB2-2DAA-4D49-A1AA-9609608D538E}" name="Tableau2" displayName="Tableau2" ref="A2:D14" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" tableBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BB731EB2-2DAA-4D49-A1AA-9609608D538E}" name="Tableau2" displayName="Tableau2" ref="A2:D14" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
   <autoFilter ref="A2:D14" xr:uid="{4DAD9DC0-ED51-4C92-BAE7-C5C07C70192A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B71CD2FB-5ACF-4E98-B694-E30B26A197E9}" name="Pièce" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{707E4B70-713D-4D73-8718-73203ABEC639}" name="Masse prévisionelle (kg)" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{A6F419B0-52E3-476E-94B3-C48F20FC0A4C}" name="Masse réelle (kg)" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{F3146788-0D29-4B0A-9648-6D7ECDD32F6F}" name="Quantité" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{B71CD2FB-5ACF-4E98-B694-E30B26A197E9}" name="Pièce" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{707E4B70-713D-4D73-8718-73203ABEC639}" name="Masse prévisionelle (kg)" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{A6F419B0-52E3-476E-94B3-C48F20FC0A4C}" name="Masse réelle (kg)" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{F3146788-0D29-4B0A-9648-6D7ECDD32F6F}" name="Quantité" dataDxfId="23"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C1488790-AB48-4066-A98E-9065D8DBABA2}" name="Tableau810" displayName="Tableau810" ref="A2:D15" totalsRowShown="0" headerRowDxfId="3" tableBorderDxfId="2">
+  <autoFilter ref="A2:D15" xr:uid="{CDFD8F50-6C62-49CB-8D1D-3EA40188DE92}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C58AF7B5-F6A6-4C80-AD90-3B1A47DD27C3}" name="Pièce"/>
+    <tableColumn id="2" xr3:uid="{0775DC2E-94C9-4C48-967C-D86444EBE01B}" name="Masse prévisionelle (kg)"/>
+    <tableColumn id="3" xr3:uid="{C94D50B6-889A-4B35-AFA8-FF8B47590CF3}" name="Masse réelle (kg)"/>
+    <tableColumn id="4" xr3:uid="{F2A95AB2-C965-4E9F-9778-8CA51E2ACA0D}" name="Quantité"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0F901C44-8085-4F13-8293-546A7DBC4743}" name="Tableau3" displayName="Tableau3" ref="A2:D11" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
-  <autoFilter ref="A2:D11" xr:uid="{1B600470-C1F9-4271-A8D4-6F8B4E21D8A7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0F901C44-8085-4F13-8293-546A7DBC4743}" name="Tableau3" displayName="Tableau3" ref="A2:D12" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
+  <autoFilter ref="A2:D12" xr:uid="{1B600470-C1F9-4271-A8D4-6F8B4E21D8A7}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C7C06F1-C1B8-402A-997E-417ED6473497}" name="Pièce" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{EEBA0232-77DC-4FF5-9D48-C226B213DB3A}" name="Masse prévisionelle (kg)" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{1B6FC5ED-303C-41ED-9F4F-2D750133D9D1}" name="Masse réelle (kg)" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{79843A3C-826C-42CA-91C0-D088717F8A80}" name="Quantité" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{8C7C06F1-C1B8-402A-997E-417ED6473497}" name="Pièce" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{EEBA0232-77DC-4FF5-9D48-C226B213DB3A}" name="Masse prévisionelle (kg)" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{1B6FC5ED-303C-41ED-9F4F-2D750133D9D1}" name="Masse réelle (kg)" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{79843A3C-826C-42CA-91C0-D088717F8A80}" name="Quantité" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5A52ADDE-DF03-49DC-B670-A05066A47047}" name="Tableau4" displayName="Tableau4" ref="A2:D10" totalsRowShown="0" headerRowDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A2:D10" xr:uid="{D4623485-F4E5-4E75-A60A-92E25E41E084}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5A52ADDE-DF03-49DC-B670-A05066A47047}" name="Tableau4" displayName="Tableau4" ref="A2:D20" totalsRowShown="0" headerRowDxfId="15" tableBorderDxfId="14">
+  <autoFilter ref="A2:D20" xr:uid="{D4623485-F4E5-4E75-A60A-92E25E41E084}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{519A70B0-70F3-4CA3-A457-62DD1A7A095C}" name="Pièce"/>
     <tableColumn id="2" xr3:uid="{B2CBC922-4F86-4CC1-91A1-E134131DCAB9}" name="Masse prévisionelle (kg)"/>
@@ -1147,7 +2981,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A2691E86-688D-47D6-B2CC-68F0AA4F0F89}" name="Tableau6" displayName="Tableau6" ref="A2:D12" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A2691E86-688D-47D6-B2CC-68F0AA4F0F89}" name="Tableau6" displayName="Tableau6" ref="A2:D12" totalsRowShown="0" headerRowDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="A2:D12" xr:uid="{330E73C6-96F5-4AE0-92E2-21EE10656014}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{28A9D6E3-A07E-4A23-B9B5-0A9B789A4839}" name="Jauge AWG"/>
@@ -1160,7 +2994,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D9EC617A-6B8C-470B-8745-D39E83718DE0}" name="Tableau68" displayName="Tableau68" ref="A2:D12" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D9EC617A-6B8C-470B-8745-D39E83718DE0}" name="Tableau68" displayName="Tableau68" ref="A2:D12" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="A2:D12" xr:uid="{20EBDB83-6F40-4F15-9054-B3BA64292F7D}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4B95F233-D697-4E5A-832D-F9AC7DA86515}" name="Jauge AWG"/>
@@ -1173,8 +3007,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BC281ED9-F434-4B3A-B0D0-16F74D98571E}" name="Tableau8" displayName="Tableau8" ref="A2:D15" totalsRowShown="0" headerRowDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A2:D15" xr:uid="{E0364261-979B-4E7C-8308-D972988CA899}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BC281ED9-F434-4B3A-B0D0-16F74D98571E}" name="Tableau8" displayName="Tableau8" ref="A2:D5" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="A2:D5" xr:uid="{E0364261-979B-4E7C-8308-D972988CA899}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C6F7D863-EB66-4E9D-8B0A-3445DB2D4FEB}" name="Pièce"/>
     <tableColumn id="2" xr3:uid="{10253E34-2D01-4EB5-A6F5-8AEE4E1D2345}" name="Masse prévisionelle (kg)"/>
@@ -1186,7 +3020,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{026F6B17-56E4-4938-AA46-9E8542536CB7}" name="Tableau82" displayName="Tableau82" ref="A2:D9" totalsRowShown="0" headerRowDxfId="5" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{026F6B17-56E4-4938-AA46-9E8542536CB7}" name="Tableau82" displayName="Tableau82" ref="A2:D9" totalsRowShown="0" headerRowDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="A2:D9" xr:uid="{C4063583-102C-40CE-909E-68F44A1DDBFD}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B379CC37-2779-4188-B921-182BFF552CB9}" name="Pièce"/>
@@ -1199,8 +3033,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F14E355-6B43-43F2-87BE-52D5B27B5B03}" name="Tableau86" displayName="Tableau86" ref="A2:D15" totalsRowShown="0" headerRowDxfId="3" tableBorderDxfId="2">
-  <autoFilter ref="A2:D15" xr:uid="{3D3FD803-42F2-4E39-8270-FBACDF8842A1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F14E355-6B43-43F2-87BE-52D5B27B5B03}" name="Tableau86" displayName="Tableau86" ref="A2:D16" totalsRowShown="0" headerRowDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A2:D16" xr:uid="{3D3FD803-42F2-4E39-8270-FBACDF8842A1}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{1C06C249-0467-423B-99AC-78BAAE27DE4C}" name="Pièce"/>
     <tableColumn id="2" xr3:uid="{AFCE3A09-E3BE-4660-BC24-5B507E8F0BF1}" name="Masse prévisionelle (kg)"/>
@@ -1212,13 +3046,13 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C1488790-AB48-4066-A98E-9065D8DBABA2}" name="Tableau810" displayName="Tableau810" ref="A2:D15" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A2:D15" xr:uid="{CDFD8F50-6C62-49CB-8D1D-3EA40188DE92}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D054D078-CB51-42B1-A955-EB8D1990C722}" name="Tableau81011" displayName="Tableau81011" ref="A2:D6" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A2:D6" xr:uid="{875CDDE8-9105-4623-8E89-1BDE3B3E4174}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C58AF7B5-F6A6-4C80-AD90-3B1A47DD27C3}" name="Pièce"/>
-    <tableColumn id="2" xr3:uid="{0775DC2E-94C9-4C48-967C-D86444EBE01B}" name="Masse prévisionelle (kg)"/>
-    <tableColumn id="3" xr3:uid="{C94D50B6-889A-4B35-AFA8-FF8B47590CF3}" name="Masse réelle (kg)"/>
-    <tableColumn id="4" xr3:uid="{F2A95AB2-C965-4E9F-9778-8CA51E2ACA0D}" name="Quantité"/>
+    <tableColumn id="1" xr3:uid="{59F5922C-0A0C-4F71-B34A-185DA9D0C142}" name="Pièce"/>
+    <tableColumn id="2" xr3:uid="{F7D4FAE5-2E56-4A1F-8CFA-1EDEA1D89A63}" name="Masse prévisionelle (kg)"/>
+    <tableColumn id="3" xr3:uid="{E0B354F0-859F-4F5A-BFEE-3F91FAC1F964}" name="Masse réelle (kg)"/>
+    <tableColumn id="4" xr3:uid="{5DF7C591-26AD-4F05-A66C-73B697FA169D}" name="Quantité"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1489,8 +3323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,13 +3339,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D1" s="11"/>
@@ -1519,133 +3353,209 @@
       <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
+      <c r="B2" s="12">
+        <f>Chapes!C15</f>
+        <v>0.11100000000000004</v>
+      </c>
+      <c r="C2" s="12">
+        <f>Chapes!C19</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
+      <c r="B3" s="12">
+        <f>'Tableau de Bord'!B13</f>
+        <v>1.0020000000000002</v>
+      </c>
+      <c r="C3" s="12">
+        <f>'Tableau de Bord'!B14</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
+      <c r="B4" s="12">
+        <f>Connecteur!C24</f>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C4" s="12">
+        <f>Chapes!C21</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
+      <c r="B5" s="50">
+        <f>'Câble faisceau arrière'!B13</f>
+        <v>0.55620000000000003</v>
+      </c>
+      <c r="C5" s="12">
+        <f>Chapes!C22</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
+      <c r="B6" s="12">
+        <f>'Câble faisceau avant'!B13</f>
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="C6" s="12">
+        <f>Chapes!C23</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
+      <c r="B7" s="12">
+        <f>'Power box'!B6</f>
+        <v>0.45499999999999996</v>
+      </c>
+      <c r="C7" s="12">
+        <f>Chapes!C24</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
+      <c r="A8" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="12">
+        <f>Télémétrie!C10</f>
+        <v>0.71500000000000008</v>
+      </c>
+      <c r="C8" s="12">
+        <f>Chapes!C25</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
+      <c r="A9" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="12">
+        <f>Autres!C17</f>
+        <v>3.8790000000000004</v>
+      </c>
+      <c r="C9" s="12">
+        <f>Chapes!C26</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
+      <c r="A10" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="12">
+        <f>Visserie!C16</f>
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="C10" s="12">
+        <f>Chapes!C27</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="12">
+        <f>'Passage de vitesse'!B7</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="C11" s="12">
+        <f>Chapes!C28</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
+      <c r="A12" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="51">
+        <f>SUM(B2:B11)</f>
+        <v>9.9812000000000012</v>
+      </c>
+      <c r="C12" s="35">
+        <f>SUM(C2:C11)</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+    <row r="16" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="34"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1939,36 +3849,194 @@
       <c r="F52" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C12:C16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F561E2-90AB-42CD-9E1B-F9BFE28F98C3}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7ECC5D-6D55-4CA5-ABBD-7BC384DED531}">
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5">
+        <v>0.4</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6">
+        <v>0.2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="41">
+        <f>SUMPRODUCT(Tableau81011[Masse prévisionelle (kg)],Tableau81011[Quantité])</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="41">
+        <f>SUMPRODUCT(Tableau2[Quantité],Tableau2[Masse réelle (kg)])</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="38"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="38"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="40"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F561E2-90AB-42CD-9E1B-F9BFE28F98C3}">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-    </row>
-    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1983,14 +4051,137 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="24">
+        <f>SUMPRODUCT(Tableau810[Masse prévisionelle (kg)],Tableau810[Quantité])</f>
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="D16" s="25"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="27"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="22"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="29"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="19"/>
+      <c r="C20" s="24">
+        <f>SUMPRODUCT(Tableau2[Quantité],Tableau2[Masse réelle (kg)])</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="25"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="27"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="27"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="22"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A16:B19"/>
+    <mergeCell ref="C16:D19"/>
+    <mergeCell ref="A20:B23"/>
+    <mergeCell ref="C20:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2003,8 +4194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E29F4E1-9C79-4318-A4EE-FFB3A483737E}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2016,12 +4207,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2183,62 +4374,62 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="25">
+      <c r="B15" s="19"/>
+      <c r="C15" s="24">
         <f>SUMPRODUCT(Tableau2[Quantité],Tableau2[Masse prévisionelle (kg)])</f>
         <v>0.11100000000000004</v>
       </c>
-      <c r="D15" s="26"/>
+      <c r="D15" s="25"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="28"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="27"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="30"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="25">
+      <c r="B19" s="19"/>
+      <c r="C19" s="24">
         <f>SUMPRODUCT(Tableau2[Quantité],Tableau2[Masse réelle (kg)])</f>
         <v>0</v>
       </c>
-      <c r="D19" s="26"/>
+      <c r="D19" s="25"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="28"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="27"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="28"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="27"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="23"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="30"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2257,27 +4448,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5A8A04-D434-438C-A29D-C19150690A4B}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.85546875" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2297,7 +4488,9 @@
       <c r="A3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3">
+        <v>0.2</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4">
         <v>1</v>
@@ -2307,126 +4500,169 @@
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1">
+        <v>0.03</v>
+      </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="6">
+        <v>0.02</v>
+      </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="D5" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="6">
+        <v>3.2000000000000001E-2</v>
+      </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="6">
+        <v>0.03</v>
+      </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="6">
+        <v>0.05</v>
+      </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="D8" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="6">
+        <v>0.05</v>
+      </c>
       <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="D9" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="6">
+        <v>0.04</v>
+      </c>
       <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.3</v>
+      </c>
       <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="28"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="28"/>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="30"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="B13" s="41">
+        <f>SUMPRODUCT(Tableau3[Masse prévisionelle (kg)],Tableau3[Quantité])</f>
+        <v>1.0020000000000002</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="25">
+      <c r="B14" s="41">
         <f>SUMPRODUCT(Tableau2[Quantité],Tableau2[Masse réelle (kg)])</f>
         <v>0</v>
       </c>
-      <c r="D16" s="26"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="28"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="40"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="40"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A12:B15"/>
-    <mergeCell ref="C12:D15"/>
-    <mergeCell ref="A16:B19"/>
-    <mergeCell ref="C16:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2437,10 +4673,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61ED984D-F746-4363-BCB8-0CD27FEF0637}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2452,14 +4688,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-    </row>
-    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -2474,14 +4710,287 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="19"/>
+      <c r="C24" s="24">
+        <f>SUMPRODUCT(Tableau4[Masse prévisionelle (kg)],Tableau4[Quantité])</f>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D24" s="25"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="20"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="27"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="27"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="22"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="29"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="19"/>
+      <c r="C28" s="24">
+        <f>SUMPRODUCT(Tableau2[Quantité],Tableau2[Masse réelle (kg)])</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="25"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="27"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="20"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="27"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="22"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A24:B27"/>
+    <mergeCell ref="C24:D27"/>
+    <mergeCell ref="A28:B31"/>
+    <mergeCell ref="C28:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2492,27 +5001,27 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A355120-A89C-4678-85B9-15FBA17DD910}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2532,31 +5041,109 @@
       <c r="A3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="4">
+        <v>3.0000000000000001E-3</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4">
-        <v>40</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
+      <c r="B4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
+      <c r="B5">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D5">
+        <v>2.1</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
+      <c r="B6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D6">
+        <v>4.2</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:4" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="49">
+        <f>SUMPRODUCT(Tableau6[Masse linéaire prévisionelle (kg/m)],Tableau6[Longueur(m)])</f>
+        <v>0.55620000000000003</v>
+      </c>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="41">
+        <f>SUMPRODUCT(Tableau2[Quantité],Tableau2[Masse réelle (kg)])</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="38"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="38"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2571,27 +5158,27 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF094D9B-C514-4FDB-B562-C839DC7B8C51}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2608,10 +5195,84 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="4">
+        <v>3.0000000000000001E-3</v>
+      </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:4" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="41">
+        <f>SUMPRODUCT(Tableau68[Masse linéaire prévisionelle (kg)],Tableau68[Longueur])</f>
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="41">
+        <f>SUMPRODUCT(Tableau2[Quantité],Tableau2[Masse réelle (kg)])</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="38"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="2"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2626,10 +5287,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B846D932-1826-4E4B-A9C7-B21858D93C14}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D15"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2641,12 +5302,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2663,10 +5324,95 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.3</v>
+      </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4">
+        <v>0.03</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="41">
+        <f>SUMPRODUCT(Tableau8[Masse prévisionelle (kg)],Tableau8[Quantité])</f>
+        <v>0.45499999999999996</v>
+      </c>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="41">
+        <f>SUMPRODUCT(Tableau2[Quantité],Tableau2[Masse réelle (kg)])</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="38"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="40"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="40"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="40"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2681,10 +5427,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7773EC5-C149-4B13-BC0D-C10B66772D1F}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2696,12 +5442,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2721,7 +5467,9 @@
       <c r="A3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="4">
+        <v>0.255</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4">
         <v>1</v>
@@ -2731,6 +5479,9 @@
       <c r="A4" t="s">
         <v>49</v>
       </c>
+      <c r="B4">
+        <v>0.09</v>
+      </c>
       <c r="D4">
         <v>2</v>
       </c>
@@ -2739,6 +5490,9 @@
       <c r="A5" t="s">
         <v>50</v>
       </c>
+      <c r="B5">
+        <v>0.06</v>
+      </c>
       <c r="D5">
         <v>2</v>
       </c>
@@ -2747,6 +5501,9 @@
       <c r="A6" t="s">
         <v>51</v>
       </c>
+      <c r="B6">
+        <v>0.06</v>
+      </c>
       <c r="D6">
         <v>1</v>
       </c>
@@ -2755,6 +5512,9 @@
       <c r="A7" t="s">
         <v>52</v>
       </c>
+      <c r="B7">
+        <v>0.06</v>
+      </c>
       <c r="D7">
         <v>1</v>
       </c>
@@ -2763,13 +5523,79 @@
       <c r="A8" t="s">
         <v>53</v>
       </c>
+      <c r="B8">
+        <v>0.04</v>
+      </c>
       <c r="D8">
         <v>1</v>
       </c>
     </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="24">
+        <f>SUMPRODUCT(Tableau82[Masse prévisionelle (kg)],Tableau82[Quantité])</f>
+        <v>0.71500000000000008</v>
+      </c>
+      <c r="D10" s="25"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="27"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="27"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="29"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="24">
+        <f>SUMPRODUCT(Tableau2[Quantité],Tableau2[Masse réelle (kg)])</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="25"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="27"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="27"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A10:B13"/>
+    <mergeCell ref="C10:D13"/>
+    <mergeCell ref="A14:B17"/>
+    <mergeCell ref="C14:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2780,27 +5606,27 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5D97A5-A601-428C-8D7C-12E0E3F8A64B}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2830,9 +5656,198 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5">
+        <v>0.1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6">
+        <v>0.15</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7">
+        <v>0.12</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <v>0.03</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9">
+        <v>0.05</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10">
+        <v>0.4</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12">
+        <v>0.02</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14">
+        <v>1.3</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="24">
+        <f>SUMPRODUCT(B3:B16,D3:D16)</f>
+        <v>3.8790000000000004</v>
+      </c>
+      <c r="D17" s="25"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="27"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="27"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="29"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="19"/>
+      <c r="C21" s="24">
+        <f>SUMPRODUCT(Tableau2[Quantité],Tableau2[Masse réelle (kg)])</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="25"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="27"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="27"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="22"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="29"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A17:B20"/>
+    <mergeCell ref="C17:D20"/>
+    <mergeCell ref="A21:B24"/>
+    <mergeCell ref="C21:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
pôle elec à 9kg qui dit mieux ?
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/Masse Elec.xlsx
+++ b/EL - Electrical/Autre/Masse Elec.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98266C2F-7CB8-493F-A70C-C9398709D40B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987E91A7-7377-498F-A632-FA4128620381}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="906" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,15 +11,14 @@
     <sheet name="TOTAL" sheetId="1" r:id="rId1"/>
     <sheet name="Chapes" sheetId="7" r:id="rId2"/>
     <sheet name="Tableau de Bord" sheetId="6" r:id="rId3"/>
-    <sheet name="Carte Avant" sheetId="12" r:id="rId4"/>
-    <sheet name="Connecteur" sheetId="5" r:id="rId5"/>
-    <sheet name="Câble faisceau arrière" sheetId="2" r:id="rId6"/>
-    <sheet name="Câble faisceau avant" sheetId="3" r:id="rId7"/>
-    <sheet name="Power box" sheetId="4" r:id="rId8"/>
-    <sheet name="Télémétrie" sheetId="8" r:id="rId9"/>
-    <sheet name="Autres" sheetId="9" r:id="rId10"/>
-    <sheet name="Passage de vitesse" sheetId="11" r:id="rId11"/>
-    <sheet name="Visserie" sheetId="10" r:id="rId12"/>
+    <sheet name="Connecteur" sheetId="5" r:id="rId4"/>
+    <sheet name="Câble faisceau arrière" sheetId="2" r:id="rId5"/>
+    <sheet name="Câble faisceau avant" sheetId="3" r:id="rId6"/>
+    <sheet name="Power box" sheetId="4" r:id="rId7"/>
+    <sheet name="Télémétrie" sheetId="8" r:id="rId8"/>
+    <sheet name="Autres" sheetId="9" r:id="rId9"/>
+    <sheet name="Passage de vitesse" sheetId="11" r:id="rId10"/>
+    <sheet name="Visserie" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="119">
   <si>
     <t>Pièce</t>
   </si>
@@ -347,15 +346,6 @@
     <t>c</t>
   </si>
   <si>
-    <t>Carte Avant</t>
-  </si>
-  <si>
-    <t>Arduino + Shield</t>
-  </si>
-  <si>
-    <t>Boite</t>
-  </si>
-  <si>
     <t xml:space="preserve">Master switch </t>
   </si>
   <si>
@@ -396,6 +386,12 @@
   </si>
   <si>
     <t>Dans les faisceau</t>
+  </si>
+  <si>
+    <t>avec le faisceau arrière</t>
+  </si>
+  <si>
+    <t>tous pesée avec les faisceau ou les boite</t>
   </si>
 </sst>
 </file>
@@ -818,6 +814,10 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -896,171 +896,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="medium">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="medium">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="medium">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="medium">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <border outline="0">
         <top style="medium">
@@ -1328,6 +1168,162 @@
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
+        <top style="medium">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="medium">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="medium">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="medium">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
         <top style="thin">
           <color theme="4"/>
         </top>
@@ -1537,8 +1533,225 @@
       <c:pieChart>
         <c:varyColors val="1"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TOTAL!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Masse prévisionelle (kg)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002B-B706-4D34-A7D4-12BC6D0031F1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002C-B706-4D34-A7D4-12BC6D0031F1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002D-B706-4D34-A7D4-12BC6D0031F1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002E-B706-4D34-A7D4-12BC6D0031F1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002F-B706-4D34-A7D4-12BC6D0031F1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000030-B706-4D34-A7D4-12BC6D0031F1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000031-B706-4D34-A7D4-12BC6D0031F1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000032-B706-4D34-A7D4-12BC6D0031F1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000033-B706-4D34-A7D4-12BC6D0031F1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000034-B706-4D34-A7D4-12BC6D0031F1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>TOTAL!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Chapes</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tableau de bord</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Connecteur</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Câbles faisceau arrière</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Câbles faisceau avant</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Power box</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Télémétrie</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Autres (DTA, Batterie..)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Visserie</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Passage de vitesse</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TOTAL!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.11100000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0220000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.000">
+                  <c:v>0.55620000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71500000000000008</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.8790000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.14499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4000000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002A-B706-4D34-A7D4-12BC6D0031F1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>TOTAL!$B$1</c:f>
@@ -1570,7 +1783,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-C149-455F-928B-59C6D903BA17}"/>
+                <c16:uniqueId val="{00000016-B706-4D34-A7D4-12BC6D0031F1}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1594,7 +1807,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000002-C149-455F-928B-59C6D903BA17}"/>
+                <c16:uniqueId val="{00000018-B706-4D34-A7D4-12BC6D0031F1}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1618,7 +1831,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-C149-455F-928B-59C6D903BA17}"/>
+                <c16:uniqueId val="{0000001A-B706-4D34-A7D4-12BC6D0031F1}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1642,7 +1855,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000004-C149-455F-928B-59C6D903BA17}"/>
+                <c16:uniqueId val="{0000001C-B706-4D34-A7D4-12BC6D0031F1}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1666,7 +1879,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-C149-455F-928B-59C6D903BA17}"/>
+                <c16:uniqueId val="{0000001E-B706-4D34-A7D4-12BC6D0031F1}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1690,7 +1903,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000006-C149-455F-928B-59C6D903BA17}"/>
+                <c16:uniqueId val="{00000020-B706-4D34-A7D4-12BC6D0031F1}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1716,7 +1929,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-C149-455F-928B-59C6D903BA17}"/>
+                <c16:uniqueId val="{00000022-B706-4D34-A7D4-12BC6D0031F1}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1742,7 +1955,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000008-C149-455F-928B-59C6D903BA17}"/>
+                <c16:uniqueId val="{00000024-B706-4D34-A7D4-12BC6D0031F1}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1768,7 +1981,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-C149-455F-928B-59C6D903BA17}"/>
+                <c16:uniqueId val="{00000026-B706-4D34-A7D4-12BC6D0031F1}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1794,7 +2007,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000A-C149-455F-928B-59C6D903BA17}"/>
+                <c16:uniqueId val="{00000028-B706-4D34-A7D4-12BC6D0031F1}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1836,7 +2049,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-C149-455F-928B-59C6D903BA17}"/>
+                  <c16:uniqueId val="{00000016-B706-4D34-A7D4-12BC6D0031F1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1877,7 +2090,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-C149-455F-928B-59C6D903BA17}"/>
+                  <c16:uniqueId val="{00000018-B706-4D34-A7D4-12BC6D0031F1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1918,7 +2131,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-C149-455F-928B-59C6D903BA17}"/>
+                  <c16:uniqueId val="{0000001A-B706-4D34-A7D4-12BC6D0031F1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1959,7 +2172,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-C149-455F-928B-59C6D903BA17}"/>
+                  <c16:uniqueId val="{0000001C-B706-4D34-A7D4-12BC6D0031F1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2000,7 +2213,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-C149-455F-928B-59C6D903BA17}"/>
+                  <c16:uniqueId val="{0000001E-B706-4D34-A7D4-12BC6D0031F1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2041,7 +2254,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-C149-455F-928B-59C6D903BA17}"/>
+                  <c16:uniqueId val="{00000020-B706-4D34-A7D4-12BC6D0031F1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2084,7 +2297,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-C149-455F-928B-59C6D903BA17}"/>
+                  <c16:uniqueId val="{00000022-B706-4D34-A7D4-12BC6D0031F1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2127,7 +2340,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-C149-455F-928B-59C6D903BA17}"/>
+                  <c16:uniqueId val="{00000024-B706-4D34-A7D4-12BC6D0031F1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2170,7 +2383,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000009-C149-455F-928B-59C6D903BA17}"/>
+                  <c16:uniqueId val="{00000026-B706-4D34-A7D4-12BC6D0031F1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2213,7 +2426,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000A-C149-455F-928B-59C6D903BA17}"/>
+                  <c16:uniqueId val="{00000028-B706-4D34-A7D4-12BC6D0031F1}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2329,7 +2542,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C149-455F-928B-59C6D903BA17}"/>
+              <c16:uniqueId val="{00000029-B706-4D34-A7D4-12BC6D0031F1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2345,6 +2558,345 @@
         </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TOTAL!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Masse réelle (kg)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>TOTAL!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Chapes</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tableau de bord</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Connecteur</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Câbles faisceau arrière</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Câbles faisceau avant</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Power box</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Télémétrie</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Autres (DTA, Batterie..)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Visserie</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Passage de vitesse</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TOTAL!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.80100000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2430000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CE5B-4EB7-AD24-812F1B85EAE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2353,6 +2905,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2438,7 +3021,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="259">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2449,7 +3032,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -2461,6 +3044,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
@@ -2484,25 +3078,29 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <cs:styleClr val="auto"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
+    <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <cs:styleClr val="auto"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2510,65 +3108,50 @@
       </a:solidFill>
       <a:ln>
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" b="1" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="20000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="10000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-      <a:scene3d>
-        <a:camera prst="orthographicFront"/>
-        <a:lightRig rig="threePt" dir="t"/>
-      </a:scene3d>
-      <a:sp3d>
-        <a:bevelT w="127000" h="127000"/>
-        <a:bevelB w="127000" h="127000"/>
-      </a:sp3d>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -2578,7 +3161,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="28575" cap="rnd">
@@ -2590,26 +3173,25 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -2617,7 +3199,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2822,7 +3404,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -2830,7 +3412,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -2874,7 +3456,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2890,7 +3472,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2995,6 +3577,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C6193BA-61F5-42AC-A664-2B7AB73E2A9E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3012,7 +3630,7 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tableau810" displayName="Tableau810" ref="A2:D15" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tableau810" displayName="Tableau810" ref="A2:D15" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A2:D15" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Pièce"/>
@@ -3025,21 +3643,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau3" displayName="Tableau3" ref="A2:D13" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau3" displayName="Tableau3" ref="A2:D13" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
   <autoFilter ref="A2:D13" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Pièce" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Masse prévisionelle (kg)" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Masse réelle (kg)" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Quantité" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Pièce" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Masse prévisionelle (kg)" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Masse réelle (kg)" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Quantité" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tableau4" displayName="Tableau4" ref="A2:D20" totalsRowShown="0" headerRowDxfId="22" tableBorderDxfId="21">
-  <autoFilter ref="A2:D20" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tableau4" displayName="Tableau4" ref="A2:D21" totalsRowShown="0" headerRowDxfId="15" tableBorderDxfId="14">
+  <autoFilter ref="A2:D21" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Pièce"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Masse prévisionelle (kg)"/>
@@ -3051,7 +3669,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau6" displayName="Tableau6" ref="A2:D12" totalsRowShown="0" headerRowDxfId="20" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau6" displayName="Tableau6" ref="A2:D12" totalsRowShown="0" headerRowDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="A2:D12" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Jauge AWG"/>
@@ -3064,7 +3682,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tableau68" displayName="Tableau68" ref="A2:D12" totalsRowShown="0" headerRowDxfId="18" tableBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tableau68" displayName="Tableau68" ref="A2:D12" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="A2:D12" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Jauge AWG"/>
@@ -3077,7 +3695,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tableau8" displayName="Tableau8" ref="A2:D5" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tableau8" displayName="Tableau8" ref="A2:D5" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="A2:D5" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Pièce"/>
@@ -3090,7 +3708,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tableau82" displayName="Tableau82" ref="A2:D9" totalsRowShown="0" headerRowDxfId="14" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tableau82" displayName="Tableau82" ref="A2:D9" totalsRowShown="0" headerRowDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="A2:D9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Pièce"/>
@@ -3103,7 +3721,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tableau86" displayName="Tableau86" ref="A2:E16" totalsRowShown="0" headerRowDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tableau86" displayName="Tableau86" ref="A2:E16" totalsRowShown="0" headerRowDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A2:E16" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Pièce"/>
@@ -3117,7 +3735,7 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tableau81011" displayName="Tableau81011" ref="A2:E6" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tableau81011" displayName="Tableau81011" ref="A2:E6" totalsRowShown="0" headerRowDxfId="3" tableBorderDxfId="2">
   <autoFilter ref="A2:E6" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Pièce"/>
@@ -3396,7 +4014,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3469,7 +4087,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="13"/>
@@ -3519,7 +4137,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
@@ -3589,14 +4207,14 @@
       <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="34">
+      <c r="B12" s="36">
         <f>SUM(B2:B11)</f>
         <v>10.8712</v>
       </c>
-      <c r="C12" s="37">
+      <c r="C12" s="39">
         <f>SUM(C2:C11)</f>
         <v>8.4440000000000008</v>
       </c>
@@ -3605,33 +4223,33 @@
       <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="38"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="38"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="40"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="38"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="40"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="33"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="39"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="41"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -3937,328 +4555,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:E25"/>
-  <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:D24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-    </row>
-    <row r="2" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="4">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="C3" s="4">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4">
-        <v>0.3</v>
-      </c>
-      <c r="C4">
-        <v>0.2</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5">
-        <v>0.1</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6">
-        <v>0.15</v>
-      </c>
-      <c r="C6">
-        <v>0.1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7">
-        <v>0.12</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8">
-        <v>0.03</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>4</v>
-      </c>
-      <c r="E8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9">
-        <v>0.05</v>
-      </c>
-      <c r="C9">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10">
-        <v>0.4</v>
-      </c>
-      <c r="C10">
-        <v>0.378</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="C11">
-        <v>0.81699999999999995</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12">
-        <v>0.02</v>
-      </c>
-      <c r="C12">
-        <v>0.1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="C13">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B14">
-        <v>1.3</v>
-      </c>
-      <c r="C14">
-        <v>1.325</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>113</v>
-      </c>
-      <c r="C16">
-        <v>0.09</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="43"/>
-      <c r="C17" s="48">
-        <f>SUMPRODUCT(B3:B16,D3:D16)</f>
-        <v>3.8790000000000004</v>
-      </c>
-      <c r="D17" s="49"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="51"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
-      <c r="B19" s="45"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="51"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="46"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="53"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="48">
-        <f>SUMPRODUCT(Tableau86[Quantité],Tableau86[Masse réelle (kg)])</f>
-        <v>3.2149999999999999</v>
-      </c>
-      <c r="D21" s="49"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
-      <c r="B23" s="45"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="51"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="46"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="53"/>
-    </row>
-    <row r="25" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A25" s="56" t="s">
-        <v>109</v>
-      </c>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56">
-        <f>C17-C21</f>
-        <v>0.66400000000000059</v>
-      </c>
-      <c r="D25" s="56"/>
-    </row>
-  </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A17:B20"/>
-    <mergeCell ref="C17:D20"/>
-    <mergeCell ref="A21:B24"/>
-    <mergeCell ref="C21:D24"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4270,12 +4571,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
     </row>
     <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -4291,7 +4592,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4321,6 +4622,9 @@
       <c r="D4">
         <v>1</v>
       </c>
+      <c r="E4" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -4350,7 +4654,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4422,7 +4726,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
@@ -4439,12 +4743,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -4528,62 +4832,62 @@
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="48">
+      <c r="B16" s="45"/>
+      <c r="C16" s="50">
         <f>SUMPRODUCT(Tableau810[Masse prévisionelle (kg)],Tableau810[Quantité])</f>
         <v>0.14499999999999999</v>
       </c>
-      <c r="D16" s="49"/>
+      <c r="D16" s="51"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="53"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="51"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="53"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="46"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="53"/>
+      <c r="A19" s="48"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="48">
+      <c r="B20" s="45"/>
+      <c r="C20" s="50">
         <f>SUMPRODUCT(Tableau2[Quantité],Tableau2[Masse réelle (kg)])</f>
         <v>0</v>
       </c>
-      <c r="D20" s="49"/>
+      <c r="D20" s="51"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
-      <c r="B21" s="45"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="51"/>
+      <c r="A21" s="46"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="53"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
+      <c r="A22" s="46"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="53"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="46"/>
-      <c r="B23" s="47"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="53"/>
+      <c r="A23" s="48"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4617,12 +4921,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4784,62 +5088,62 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="48">
+      <c r="B15" s="45"/>
+      <c r="C15" s="50">
         <f>SUMPRODUCT(Tableau2[Quantité],Tableau2[Masse prévisionelle (kg)])</f>
         <v>0.11100000000000004</v>
       </c>
-      <c r="D15" s="49"/>
+      <c r="D15" s="51"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="51"/>
+      <c r="A16" s="46"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="53"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="53"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="46"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="53"/>
+      <c r="A18" s="48"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="55"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="48">
+      <c r="B19" s="45"/>
+      <c r="C19" s="50">
         <f>SUMPRODUCT(Tableau2[Quantité],Tableau2[Masse réelle (kg)])</f>
         <v>0</v>
       </c>
-      <c r="D19" s="49"/>
+      <c r="D19" s="51"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
-      <c r="B20" s="45"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="51"/>
+      <c r="A20" s="46"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="53"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
-      <c r="B21" s="45"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="51"/>
+      <c r="A21" s="46"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="53"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="46"/>
-      <c r="B22" s="47"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="53"/>
+      <c r="A22" s="48"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4873,12 +5177,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
     </row>
     <row r="2" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -4948,7 +5252,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -5021,7 +5325,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5037,20 +5341,20 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="57">
+      <c r="B13" s="31">
         <v>0.02</v>
       </c>
-      <c r="C13" s="57">
+      <c r="C13" s="31">
         <v>1.9E-2</v>
       </c>
-      <c r="D13" s="58">
+      <c r="D13" s="32">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5121,72 +5425,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3">
-        <v>7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4">
-        <v>0.2</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -5199,12 +5441,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -5436,64 +5678,69 @@
         <v>21</v>
       </c>
     </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>118</v>
+      </c>
+    </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="48">
+      <c r="B24" s="45"/>
+      <c r="C24" s="50">
         <f>SUMPRODUCT(Tableau4[Masse prévisionelle (kg)],Tableau4[Quantité])</f>
         <v>1.4500000000000002</v>
       </c>
-      <c r="D24" s="49"/>
+      <c r="D24" s="51"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
-      <c r="B25" s="45"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="51"/>
+      <c r="A25" s="46"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="53"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="51"/>
+      <c r="A26" s="46"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="53"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="46"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="53"/>
+      <c r="A27" s="48"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="55"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="48">
+      <c r="B28" s="45"/>
+      <c r="C28" s="50">
         <f>SUMPRODUCT(Tableau2[Quantité],Tableau2[Masse réelle (kg)])</f>
         <v>0</v>
       </c>
-      <c r="D28" s="49"/>
+      <c r="D28" s="51"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
-      <c r="B29" s="45"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="51"/>
+      <c r="A29" s="46"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="53"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
-      <c r="B30" s="45"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="51"/>
+      <c r="A30" s="46"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="53"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="46"/>
-      <c r="B31" s="47"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="53"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5510,7 +5757,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
@@ -5527,12 +5774,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -5600,7 +5847,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C9">
         <v>1.647</v>
@@ -5608,7 +5855,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C10">
         <v>0.97299999999999998</v>
@@ -5683,7 +5930,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
@@ -5700,12 +5947,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -5746,7 +5993,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C5">
         <v>0.33</v>
@@ -5823,7 +6070,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -5840,12 +6087,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -5969,7 +6216,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -5986,12 +6233,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -6081,62 +6328,62 @@
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="48">
+      <c r="B10" s="45"/>
+      <c r="C10" s="50">
         <f>SUMPRODUCT(Tableau82[Masse prévisionelle (kg)],Tableau82[Quantité])</f>
         <v>0.71500000000000008</v>
       </c>
-      <c r="D10" s="49"/>
+      <c r="D10" s="51"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="51"/>
+      <c r="A11" s="46"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="53"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="51"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="53"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="46"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="53"/>
+      <c r="A13" s="48"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="55"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="48">
+      <c r="B14" s="45"/>
+      <c r="C14" s="50">
         <f>SUMPRODUCT(Tableau82[Masse réelle (kg)],Tableau82[Quantité])</f>
         <v>0.23499999999999999</v>
       </c>
-      <c r="D14" s="49"/>
+      <c r="D14" s="51"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="51"/>
+      <c r="A15" s="46"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="53"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="51"/>
+      <c r="A16" s="46"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="53"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="46"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="53"/>
+      <c r="A17" s="48"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6151,4 +6398,321 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="4">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+      <c r="C4">
+        <v>0.2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6">
+        <v>0.15</v>
+      </c>
+      <c r="C6">
+        <v>0.1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7">
+        <v>0.12</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8">
+        <v>0.03</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9">
+        <v>0.05</v>
+      </c>
+      <c r="C9">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10">
+        <v>0.4</v>
+      </c>
+      <c r="C10">
+        <v>0.378</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="C11">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12">
+        <v>0.02</v>
+      </c>
+      <c r="C12">
+        <v>0.1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="C13">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14">
+        <v>1.3</v>
+      </c>
+      <c r="C14">
+        <v>1.325</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16">
+        <v>0.09</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="45"/>
+      <c r="C17" s="50">
+        <f>SUMPRODUCT(B3:B16,D3:D16)</f>
+        <v>3.8790000000000004</v>
+      </c>
+      <c r="D17" s="51"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="46"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="53"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="46"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="53"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="48"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="55"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="45"/>
+      <c r="C21" s="50">
+        <f>SUMPRODUCT(Tableau86[Quantité],Tableau86[Masse réelle (kg)])</f>
+        <v>3.2149999999999999</v>
+      </c>
+      <c r="D21" s="51"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="46"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="53"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="46"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="53"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="48"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="55"/>
+    </row>
+    <row r="25" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A25" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="58"/>
+      <c r="C25" s="58">
+        <f>C17-C21</f>
+        <v>0.66400000000000059</v>
+      </c>
+      <c r="D25" s="58"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A17:B20"/>
+    <mergeCell ref="C17:D20"/>
+    <mergeCell ref="A21:B24"/>
+    <mergeCell ref="C21:D24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>